<commit_message>
Test Extraction on Git ✨ 30 ธ.ค. 63 เวลา 21:52
</commit_message>
<xml_diff>
--- a/Recent 14Days Alert Data🔥/xlsx/covid-tracker-week.xlsx
+++ b/Recent 14Days Alert Data🔥/xlsx/covid-tracker-week.xlsx
@@ -364,7 +364,7 @@
     <t>ศูนย์การแพทย์กาญจนาภิเษก อ.พุทธมณฑล</t>
   </si>
   <si>
-    <t>ตลาดท่าข้าม</t>
+    <t>ตลาดท่าข้าม อ.นครชัยศรี</t>
   </si>
   <si>
     <t>ตลาดปฐมมงคล</t>
@@ -5520,7 +5520,7 @@
         <v>152</v>
       </c>
       <c r="B100" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C100" s="2">
         <v>44189</v>
@@ -5529,10 +5529,10 @@
         <v>116</v>
       </c>
       <c r="E100">
-        <v>13.65357633</v>
+        <v>13.8017434</v>
       </c>
       <c r="F100">
-        <v>100.4481482</v>
+        <v>100.1879465</v>
       </c>
       <c r="G100">
         <v>0</v>

</xml_diff>